<commit_message>
[1.3.2] Cập nhật CSDL & Server
- Thêm khu vực nhập vị trí hàng ngang xuất hiện theo như file excel cơ sở dữ liệu trên trang web
- Điều chỉnh UI của web /database
- Thêm thông báo refresh trong trường hợp server phải khởi động lại cho user
</commit_message>
<xml_diff>
--- a/Database/Database1.xlsx
+++ b/Database/Database1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2. O Project\O_WebServerEdition\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2. O Project\Olympia_24\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306AC5C5-2C87-4B6D-BC2F-B85BB252A995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F1AA60-1FCE-43F9-B3D9-6823295FD732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D1E2E1B2-ECC6-431A-9DB1-D10D877A3DFD}"/>
+    <workbookView xWindow="4425" yWindow="1980" windowWidth="23190" windowHeight="11295" xr2:uid="{D1E2E1B2-ECC6-431A-9DB1-D10D877A3DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -2315,7 +2315,7 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -3300,7 +3300,7 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[1.3.4] Cập nhật Player và Server
- Cho phép tuỳ chỉnh việc nộp đáp án rỗng
- Thay đổi logic của cơ chế ra/vào phòng chơi
- Cập nhật thông tin tên và điểm của player vào CSDL
</commit_message>
<xml_diff>
--- a/Database/Database1.xlsx
+++ b/Database/Database1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2. O Project\Olympia_24\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2. O Project\O_WebServerEdition\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F1AA60-1FCE-43F9-B3D9-6823295FD732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5FDE1D-B916-435A-9733-FB8A5940D43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="1980" windowWidth="23190" windowHeight="11295" xr2:uid="{D1E2E1B2-ECC6-431A-9DB1-D10D877A3DFD}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{D1E2E1B2-ECC6-431A-9DB1-D10D877A3DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Acceleration" sheetId="3" r:id="rId3"/>
     <sheet name="Finish" sheetId="4" r:id="rId4"/>
     <sheet name="Sub Finish" sheetId="5" r:id="rId5"/>
+    <sheet name="Match Data" sheetId="6" r:id="rId6"/>
+    <sheet name="Match Log" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>STT</t>
   </si>
@@ -613,16 +615,56 @@
   <si>
     <t>./Acceleration/training_match_3/TT4.mp4</t>
   </si>
+  <si>
+    <t>Tên thí sinh</t>
+  </si>
+  <si>
+    <t>Điểm KĐ</t>
+  </si>
+  <si>
+    <t>Điểm VCNV</t>
+  </si>
+  <si>
+    <t>Điểm TT</t>
+  </si>
+  <si>
+    <t>Điểm VĐ</t>
+  </si>
+  <si>
+    <t>Tổng</t>
+  </si>
+  <si>
+    <t>TS1</t>
+  </si>
+  <si>
+    <t>TS2</t>
+  </si>
+  <si>
+    <t>TS3</t>
+  </si>
+  <si>
+    <t>TS4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4725</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts/>
+  <fonts x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -647,8 +689,19 @@
       <name val="Montserrat"/>
       <charset val="163"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills>
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -686,7 +739,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="65">
+  <borders>
     <border>
       <left/>
       <right/>
@@ -1594,11 +1647,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1948,6 +2027,85 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2313,739 +2471,666 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="18.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="56.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="36" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.75" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.75" style="75" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" style="75" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s" s="5">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" t="s" s="73">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2" s="118">
+    <row r="2" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A2" s="145">
         <v>1</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" t="s" s="17">
         <v>85</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" t="s" s="18">
         <v>86</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" t="s" s="19">
         <v>87</v>
       </c>
       <c r="F2" s="15"/>
-      <c r="G2" s="37" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A3" s="119"/>
+      <c r="G2" s="37"/>
+    </row>
+    <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A3" s="146"/>
       <c r="B3" s="14">
         <v>2</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" t="s" s="20">
         <v>88</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" t="s" s="21">
         <v>89</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" t="s" s="22">
         <v>90</v>
       </c>
       <c r="F3" s="16"/>
-      <c r="G3" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="119"/>
+      <c r="G3" s="35"/>
+    </row>
+    <row r="4" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A4" s="146"/>
       <c r="B4" s="14">
         <v>3</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" t="s" s="20">
         <v>91</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" t="s" s="21">
         <v>92</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" t="s" s="22">
         <v>93</v>
       </c>
       <c r="F4" s="16"/>
-      <c r="G4" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="54" x14ac:dyDescent="0.2">
-      <c r="A5" s="119"/>
+      <c r="G4" s="35"/>
+    </row>
+    <row r="5" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+      <c r="A5" s="146"/>
       <c r="B5" s="14">
         <v>4</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" t="s" s="20">
         <v>94</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" t="s" s="21">
         <v>95</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" t="s" s="22">
         <v>96</v>
       </c>
       <c r="F5" s="16"/>
-      <c r="G5" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="119"/>
+      <c r="G5" s="35"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="146"/>
       <c r="B6" s="14">
         <v>5</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" t="s" s="20">
         <v>97</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" t="s" s="21">
         <v>98</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" t="s" s="22">
         <v>99</v>
       </c>
       <c r="F6" s="16"/>
-      <c r="G6" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="119"/>
+      <c r="G6" s="35"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="146"/>
       <c r="B7" s="14">
         <v>6</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" t="s" s="20">
         <v>100</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" t="s" s="21">
         <v>101</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" t="s" s="22">
         <v>102</v>
       </c>
       <c r="F7" s="16"/>
-      <c r="G7" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A8" s="120">
+      <c r="G7" s="35"/>
+    </row>
+    <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A8" s="147">
         <v>2</v>
       </c>
       <c r="B8" s="23">
         <v>1</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" t="s" s="25">
         <v>94</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" t="s" s="26">
         <v>103</v>
       </c>
-      <c r="E8" s="25" t="s">
-        <v>104</v>
+      <c r="E8" s="25">
+        <v>0</v>
       </c>
       <c r="F8" s="24"/>
-      <c r="G8" s="41" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="120"/>
+      <c r="G8" s="41"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="147"/>
       <c r="B9" s="14">
         <v>2</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" t="s" s="27">
         <v>97</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" t="s" s="28">
         <v>105</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" t="s" s="27">
         <v>106</v>
       </c>
       <c r="F9" s="16"/>
-      <c r="G9" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A10" s="120"/>
+      <c r="G9" s="35"/>
+    </row>
+    <row r="10" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A10" s="147"/>
       <c r="B10" s="14">
         <v>3</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" t="s" s="27">
         <v>107</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" t="s" s="28">
         <v>108</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" t="s" s="27">
         <v>109</v>
       </c>
       <c r="F10" s="16"/>
-      <c r="G10" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A11" s="120"/>
+      <c r="G10" s="35"/>
+    </row>
+    <row r="11" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A11" s="147"/>
       <c r="B11" s="14">
         <v>4</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" t="s" s="27">
         <v>110</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" t="s" s="28">
         <v>111</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>19</v>
+      <c r="E11" s="27">
+        <v>5</v>
       </c>
       <c r="F11" s="16"/>
-      <c r="G11" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A12" s="120"/>
+      <c r="G11" s="35"/>
+    </row>
+    <row r="12" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A12" s="147"/>
       <c r="B12" s="14">
         <v>5</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" t="s" s="27">
         <v>100</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" t="s" s="28">
         <v>112</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" t="s" s="27">
         <v>113</v>
       </c>
       <c r="F12" s="16"/>
-      <c r="G12" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="54" x14ac:dyDescent="0.2">
-      <c r="A13" s="120"/>
+      <c r="G12" s="35"/>
+    </row>
+    <row r="13" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+      <c r="A13" s="147"/>
       <c r="B13" s="14">
         <v>6</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" t="s" s="27">
         <v>114</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" t="s" s="28">
         <v>115</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" t="s" s="27">
         <v>116</v>
       </c>
       <c r="F13" s="16"/>
-      <c r="G13" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A14" s="120">
+      <c r="G13" s="35"/>
+    </row>
+    <row r="14" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A14" s="147">
         <v>3</v>
       </c>
       <c r="B14" s="23">
         <v>1</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" t="s" s="25">
         <v>88</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" t="s" s="26">
         <v>117</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" t="s" s="25">
         <v>118</v>
       </c>
       <c r="F14" s="24"/>
-      <c r="G14" s="41" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="120"/>
+      <c r="G14" s="41"/>
+    </row>
+    <row r="15" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A15" s="147"/>
       <c r="B15" s="14">
         <v>2</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" t="s" s="27">
         <v>119</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" t="s" s="28">
         <v>120</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" t="s" s="27">
         <v>121</v>
       </c>
       <c r="F15" s="16"/>
-      <c r="G15" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="120"/>
+      <c r="G15" s="35"/>
+    </row>
+    <row r="16" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A16" s="147"/>
       <c r="B16" s="14">
         <v>3</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" t="s" s="27">
         <v>97</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" t="s" s="28">
         <v>122</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" t="s" s="27">
         <v>123</v>
       </c>
       <c r="F16" s="16"/>
-      <c r="G16" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A17" s="120"/>
+      <c r="G16" s="35"/>
+    </row>
+    <row r="17" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A17" s="147"/>
       <c r="B17" s="14">
         <v>4</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" t="s" s="27">
         <v>85</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" t="s" s="28">
         <v>124</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" t="s" s="27">
         <v>125</v>
       </c>
       <c r="F17" s="16"/>
-      <c r="G17" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A18" s="120"/>
+      <c r="G17" s="35"/>
+    </row>
+    <row r="18" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+      <c r="A18" s="147"/>
       <c r="B18" s="14">
         <v>5</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" t="s" s="27">
         <v>126</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" t="s" s="28">
         <v>127</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" t="s" s="27">
         <v>128</v>
       </c>
       <c r="F18" s="16"/>
-      <c r="G18" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="54" x14ac:dyDescent="0.2">
-      <c r="A19" s="120"/>
+      <c r="G18" s="35"/>
+    </row>
+    <row r="19" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+      <c r="A19" s="147"/>
       <c r="B19" s="14">
         <v>6</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" t="s" s="27">
         <v>110</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" t="s" s="28">
         <v>129</v>
       </c>
-      <c r="E19" s="27" t="s">
-        <v>130</v>
+      <c r="E19" s="27">
+        <v>18</v>
       </c>
       <c r="F19" s="16"/>
-      <c r="G19" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A20" s="120">
+      <c r="G19" s="35"/>
+    </row>
+    <row r="20" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A20" s="147">
         <v>4</v>
       </c>
       <c r="B20" s="23">
         <v>1</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" t="s" s="29">
         <v>119</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" t="s" s="30">
         <v>131</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" t="s" s="29">
         <v>132</v>
       </c>
       <c r="F20" s="24"/>
-      <c r="G20" s="41" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A21" s="120"/>
+      <c r="G20" s="41"/>
+    </row>
+    <row r="21" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A21" s="147"/>
       <c r="B21" s="14">
         <v>2</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" t="s" s="31">
         <v>114</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" t="s" s="21">
         <v>133</v>
       </c>
-      <c r="E21" s="31" t="s">
-        <v>134</v>
+      <c r="E21" s="31">
+        <v>7</v>
       </c>
       <c r="F21" s="16"/>
-      <c r="G21" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A22" s="120"/>
+      <c r="G21" s="35"/>
+    </row>
+    <row r="22" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+      <c r="A22" s="147"/>
       <c r="B22" s="14">
         <v>3</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" t="s" s="31">
         <v>88</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" t="s" s="21">
         <v>135</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" t="s" s="31">
         <v>136</v>
       </c>
       <c r="F22" s="16"/>
-      <c r="G22" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A23" s="120"/>
+      <c r="G22" s="35"/>
+    </row>
+    <row r="23" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A23" s="147"/>
       <c r="B23" s="14">
         <v>4</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" t="s" s="31">
         <v>126</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D23" t="s" s="21">
         <v>137</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" t="s" s="31">
         <v>138</v>
       </c>
       <c r="F23" s="16"/>
-      <c r="G23" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A24" s="120"/>
+      <c r="G23" s="35"/>
+    </row>
+    <row r="24" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+      <c r="A24" s="147"/>
       <c r="B24" s="14">
         <v>5</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" t="s" s="31">
         <v>91</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" t="s" s="21">
         <v>139</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" t="s" s="31">
         <v>140</v>
       </c>
       <c r="F24" s="16"/>
-      <c r="G24" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="121"/>
+      <c r="G24" s="35"/>
+    </row>
+    <row r="25" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A25" s="148"/>
       <c r="B25" s="88">
         <v>6</v>
       </c>
-      <c r="C25" s="89" t="s">
+      <c r="C25" t="s" s="89">
         <v>94</v>
       </c>
-      <c r="D25" s="90" t="s">
+      <c r="D25" t="s" s="90">
         <v>141</v>
       </c>
-      <c r="E25" s="89" t="s">
+      <c r="E25" t="s" s="89">
         <v>142</v>
       </c>
       <c r="F25" s="91"/>
-      <c r="G25" s="74" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="122">
+      <c r="G25" s="74"/>
+    </row>
+    <row r="26" spans="1:7" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="149">
         <v>5</v>
       </c>
       <c r="B26" s="108">
         <v>1</v>
       </c>
-      <c r="C26" s="115" t="s">
+      <c r="C26" t="s" s="115">
         <v>107</v>
       </c>
-      <c r="D26" s="109" t="s">
+      <c r="D26" t="s" s="109">
         <v>143</v>
       </c>
-      <c r="E26" s="115" t="s">
+      <c r="E26" t="s" s="115">
         <v>144</v>
       </c>
       <c r="F26" s="109"/>
-      <c r="G26" s="92" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A27" s="123"/>
+      <c r="G26" s="92"/>
+    </row>
+    <row r="27" spans="1:7" s="75" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="A27" s="150"/>
       <c r="B27" s="110">
         <v>2</v>
       </c>
-      <c r="C27" s="116" t="s">
+      <c r="C27" t="s" s="116">
         <v>119</v>
       </c>
-      <c r="D27" s="111" t="s">
+      <c r="D27" t="s" s="111">
         <v>145</v>
       </c>
-      <c r="E27" s="116" t="s">
+      <c r="E27" t="s" s="116">
         <v>146</v>
       </c>
       <c r="F27" s="111"/>
-      <c r="G27" s="93" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A28" s="123"/>
+      <c r="G27" s="93"/>
+    </row>
+    <row r="28" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A28" s="150"/>
       <c r="B28" s="110">
         <v>3</v>
       </c>
-      <c r="C28" s="116" t="s">
+      <c r="C28" t="s" s="116">
         <v>110</v>
       </c>
-      <c r="D28" s="111" t="s">
+      <c r="D28" t="s" s="111">
         <v>147</v>
       </c>
-      <c r="E28" s="116" t="s">
+      <c r="E28" t="s" s="116">
         <v>148</v>
       </c>
       <c r="F28" s="111"/>
-      <c r="G28" s="93" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="75" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A29" s="123"/>
+      <c r="G28" s="93"/>
+    </row>
+    <row r="29" spans="1:7" s="75" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="A29" s="150"/>
       <c r="B29" s="110">
         <v>4</v>
       </c>
-      <c r="C29" s="116" t="s">
+      <c r="C29" t="s" s="116">
         <v>126</v>
       </c>
-      <c r="D29" s="111" t="s">
+      <c r="D29" t="s" s="111">
         <v>149</v>
       </c>
-      <c r="E29" s="116" t="s">
+      <c r="E29" t="s" s="116">
         <v>150</v>
       </c>
       <c r="F29" s="111"/>
-      <c r="G29" s="93" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A30" s="123"/>
+      <c r="G29" s="93"/>
+    </row>
+    <row r="30" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A30" s="150"/>
       <c r="B30" s="110">
         <v>5</v>
       </c>
-      <c r="C30" s="116" t="s">
+      <c r="C30" t="s" s="116">
         <v>114</v>
       </c>
-      <c r="D30" s="111" t="s">
+      <c r="D30" t="s" s="111">
         <v>151</v>
       </c>
-      <c r="E30" s="116" t="s">
+      <c r="E30" t="s" s="116">
         <v>152</v>
       </c>
       <c r="F30" s="111"/>
-      <c r="G30" s="93" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A31" s="123"/>
+      <c r="G30" s="93"/>
+    </row>
+    <row r="31" spans="1:7" s="75" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="A31" s="150"/>
       <c r="B31" s="110">
         <v>6</v>
       </c>
-      <c r="C31" s="116" t="s">
+      <c r="C31" t="s" s="116">
         <v>126</v>
       </c>
-      <c r="D31" s="111" t="s">
+      <c r="D31" t="s" s="111">
         <v>153</v>
       </c>
-      <c r="E31" s="116" t="s">
+      <c r="E31" t="s" s="116">
         <v>154</v>
       </c>
       <c r="F31" s="111"/>
-      <c r="G31" s="93" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="75" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A32" s="123"/>
+      <c r="G31" s="93"/>
+    </row>
+    <row r="32" spans="1:7" s="75" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="A32" s="150"/>
       <c r="B32" s="112">
         <v>7</v>
       </c>
-      <c r="C32" s="116" t="s">
+      <c r="C32" t="s" s="116">
         <v>114</v>
       </c>
-      <c r="D32" s="111" t="s">
+      <c r="D32" t="s" s="111">
         <v>155</v>
       </c>
-      <c r="E32" s="116" t="s">
+      <c r="E32" t="s" s="116">
         <v>156</v>
       </c>
       <c r="F32" s="111"/>
-      <c r="G32" s="93" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A33" s="123"/>
+      <c r="G32" s="93"/>
+    </row>
+    <row r="33" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A33" s="150"/>
       <c r="B33" s="112">
         <v>8</v>
       </c>
-      <c r="C33" s="116" t="s">
+      <c r="C33" t="s" s="116">
         <v>107</v>
       </c>
-      <c r="D33" s="111" t="s">
+      <c r="D33" t="s" s="111">
         <v>157</v>
       </c>
-      <c r="E33" s="116" t="s">
+      <c r="E33" t="s" s="116">
         <v>158</v>
       </c>
       <c r="F33" s="111"/>
-      <c r="G33" s="93" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A34" s="123"/>
+      <c r="G33" s="93"/>
+    </row>
+    <row r="34" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A34" s="150"/>
       <c r="B34" s="112">
         <v>9</v>
       </c>
-      <c r="C34" s="116" t="s">
+      <c r="C34" t="s" s="116">
         <v>94</v>
       </c>
-      <c r="D34" s="111" t="s">
+      <c r="D34" t="s" s="111">
         <v>159</v>
       </c>
-      <c r="E34" s="116" t="s">
+      <c r="E34" t="s" s="116">
         <v>160</v>
       </c>
       <c r="F34" s="111"/>
-      <c r="G34" s="93" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A35" s="123"/>
+      <c r="G34" s="93"/>
+    </row>
+    <row r="35" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A35" s="150"/>
       <c r="B35" s="112">
         <v>10</v>
       </c>
-      <c r="C35" s="116" t="s">
+      <c r="C35" t="s" s="116">
         <v>88</v>
       </c>
-      <c r="D35" s="111" t="s">
+      <c r="D35" t="s" s="111">
         <v>161</v>
       </c>
-      <c r="E35" s="116" t="s">
+      <c r="E35" t="s" s="116">
         <v>162</v>
       </c>
       <c r="F35" s="111"/>
-      <c r="G35" s="93" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="75" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A36" s="123"/>
+      <c r="G35" s="93"/>
+    </row>
+    <row r="36" spans="1:7" s="75" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="A36" s="150"/>
       <c r="B36" s="112">
         <v>11</v>
       </c>
-      <c r="C36" s="116" t="s">
+      <c r="C36" t="s" s="116">
         <v>91</v>
       </c>
-      <c r="D36" s="111" t="s">
+      <c r="D36" t="s" s="111">
         <v>163</v>
       </c>
-      <c r="E36" s="116" t="s">
+      <c r="E36" t="s" s="116">
         <v>164</v>
       </c>
       <c r="F36" s="111"/>
-      <c r="G36" s="93" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="75" customFormat="1" ht="54.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="124"/>
+      <c r="G36" s="93"/>
+    </row>
+    <row r="37" spans="1:7" s="75" customFormat="1" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="151"/>
       <c r="B37" s="113">
         <v>12</v>
       </c>
-      <c r="C37" s="117" t="s">
+      <c r="C37" t="s" s="117">
         <v>85</v>
       </c>
-      <c r="D37" s="114" t="s">
+      <c r="D37" t="s" s="114">
         <v>165</v>
       </c>
-      <c r="E37" s="117" t="s">
+      <c r="E37" t="s" s="117">
         <v>166</v>
       </c>
       <c r="F37" s="114"/>
-      <c r="G37" s="94" t="s">
-        <v>167</v>
-      </c>
+      <c r="G37" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3065,226 +3150,211 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="55.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="36.75" style="2" customWidth="1"/>
-    <col min="5" max="6" width="39.25" style="2" customWidth="1"/>
+    <col min="1" max="2" width="18.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="39.28515625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="45">
         <v>7</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" t="s" s="46">
         <v>10</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" t="s" s="47">
         <v>2</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" t="s" s="48">
         <v>3</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" t="s" s="48">
         <v>4</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" t="s" s="49">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="54" x14ac:dyDescent="0.25">
       <c r="A2" s="50">
         <v>1</v>
       </c>
       <c r="B2" s="69">
         <f>LEN(SUBSTITUTE(D2," ",""))</f>
-        <v>1</v>
-      </c>
-      <c r="C2" s="51" t="s">
+      </c>
+      <c r="C2" t="s" s="51">
         <v>20</v>
       </c>
-      <c r="D2" s="40" t="s">
-        <v>18</v>
+      <c r="D2" s="40">
+        <v>6</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="108" x14ac:dyDescent="0.25">
       <c r="A3" s="52">
         <v>2</v>
       </c>
       <c r="B3" s="70">
         <f>LEN(SUBSTITUTE(D3," ",""))</f>
-        <v>14</v>
-      </c>
-      <c r="C3" s="53" t="s">
+      </c>
+      <c r="C3" t="s" s="53">
         <v>23</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" t="s" s="31">
         <v>24</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="54" x14ac:dyDescent="0.25">
       <c r="A4" s="52">
         <v>3</v>
       </c>
       <c r="B4" s="70">
         <f t="shared" ref="B4:B7" si="0">LEN(SUBSTITUTE(D4," ",""))</f>
-        <v>4</v>
-      </c>
-      <c r="C4" s="53" t="s">
+      </c>
+      <c r="C4" t="s" s="53">
         <v>21</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" t="s" s="56">
         <v>22</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="54" x14ac:dyDescent="0.25">
       <c r="A5" s="52">
         <v>4</v>
       </c>
       <c r="B5" s="70">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C5" s="53" t="s">
+      </c>
+      <c r="C5" t="s" s="53">
         <v>25</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" t="s" s="31">
         <v>26</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" ht="54" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="54" x14ac:dyDescent="0.25">
       <c r="A6" s="52">
         <v>5</v>
       </c>
       <c r="B6" s="70">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C6" s="53" t="s">
+      </c>
+      <c r="C6" t="s" s="53">
         <v>27</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" t="s" s="31">
         <v>28</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
+    <row r="7" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s" s="54">
         <v>8</v>
       </c>
       <c r="B7" s="71">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C7" s="55" t="s">
+      </c>
+      <c r="C7" t="s" s="55">
         <v>11</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" t="s" s="10">
         <v>29</v>
       </c>
       <c r="E7" s="11"/>
-      <c r="F7" s="12" t="s">
+      <c r="F7" t="s" s="12">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="s">
+    <row r="9" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s" s="72">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+    <row r="10" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s" s="47">
         <v>13</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" t="s" s="48">
         <v>14</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" t="s" s="48">
         <v>15</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" t="s" s="49">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="96">
         <v>1</v>
       </c>
       <c r="B11" s="97">
         <v>9</v>
       </c>
-      <c r="C11" s="98" t="str">
+      <c r="C11" s="98">
         <f>IF(AND(B2 + B11 - 1 &lt;= 18, B11 &gt; 0), "Hợp lệ", "Không hợp lệ")</f>
-        <v>Hợp lệ</v>
       </c>
       <c r="D11" s="99">
         <f>IF(INT((18-B2)/2 + 1) &gt; 0, INT((18-B2)/2 + 1), "undefined")</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="100">
         <v>2</v>
       </c>
       <c r="B12" s="101">
         <v>3</v>
       </c>
-      <c r="C12" s="102" t="str">
+      <c r="C12" s="102">
         <f>IF(AND(B3 + B12 - 1 &lt;= 18, B12 &gt; 0), "Hợp lệ", "Không hợp lệ")</f>
-        <v>Hợp lệ</v>
       </c>
       <c r="D12" s="103">
         <f t="shared" ref="D12:D14" si="1">IF(INT((18-B3)/2 + 1) &gt; 0, INT((18-B3)/2 + 1), "undefined")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="100">
         <v>3</v>
       </c>
       <c r="B13" s="101">
         <v>8</v>
       </c>
-      <c r="C13" s="102" t="str">
+      <c r="C13" s="102">
         <f>IF(AND(B4 + B13 - 1 &lt;= 18, B13 &gt; 0), "Hợp lệ", "Không hợp lệ")</f>
-        <v>Hợp lệ</v>
       </c>
       <c r="D13" s="103">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="104">
         <v>4</v>
       </c>
       <c r="B14" s="105">
         <v>6</v>
       </c>
-      <c r="C14" s="106" t="str">
+      <c r="C14" s="106">
         <f>IF(AND(B5 + B14 - 1 &lt;= 18, B14 &gt; 0), "Hợp lệ", "Không hợp lệ")</f>
-        <v>Hợp lệ</v>
       </c>
       <c r="D14" s="107">
         <f t="shared" si="1"/>
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3298,41 +3368,40 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" style="3"/>
     <col min="2" max="2" width="34" style="3" customWidth="1"/>
-    <col min="3" max="4" width="35.125" style="3" customWidth="1"/>
-    <col min="5" max="7" width="35.25" style="3" customWidth="1"/>
+    <col min="3" max="4" width="35.140625" style="3" customWidth="1"/>
+    <col min="5" max="7" width="35.28515625" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="76" t="s">
+      <c r="A1" t="s" s="76">
         <v>0</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" t="s" s="77">
         <v>2</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" t="s" s="78">
         <v>3</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" t="s" s="78">
         <v>12</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" t="s" s="78">
         <v>4</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="F1" t="s" s="87">
         <v>5</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="G1" t="s" s="79">
         <v>83</v>
       </c>
       <c r="H1" s="75"/>
@@ -3341,20 +3410,20 @@
       <c r="A2" s="80">
         <v>1</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" t="s" s="51">
         <v>168</v>
       </c>
-      <c r="C2" s="81" t="s">
-        <v>169</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="81">
+        <v>258258</v>
+      </c>
+      <c r="D2" t="s" s="18">
         <v>170</v>
       </c>
       <c r="E2" s="18"/>
-      <c r="F2" s="37" t="s">
+      <c r="F2" t="s" s="37">
         <v>171</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" t="s" s="37">
         <v>172</v>
       </c>
       <c r="H2" s="75"/>
@@ -3363,42 +3432,40 @@
       <c r="A3" s="82">
         <v>2</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" t="s" s="53">
         <v>173</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" t="s" s="83">
         <v>174</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" t="s" s="21">
         <v>175</v>
       </c>
       <c r="E3" s="21"/>
-      <c r="F3" s="35" t="s">
+      <c r="F3" t="s" s="35">
         <v>182</v>
       </c>
-      <c r="G3" s="35" t="s">
-        <v>167</v>
-      </c>
+      <c r="G3" s="35"/>
       <c r="H3" s="75"/>
     </row>
-    <row r="4" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="54" x14ac:dyDescent="0.35">
       <c r="A4" s="82">
         <v>3</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" t="s" s="53">
         <v>176</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" t="s" s="83">
         <v>177</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" t="s" s="21">
         <v>170</v>
       </c>
       <c r="E4" s="21"/>
-      <c r="F4" s="35" t="s">
+      <c r="F4" t="s" s="35">
         <v>178</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" t="s" s="35">
         <v>179</v>
       </c>
       <c r="H4" s="75"/>
@@ -3407,22 +3474,20 @@
       <c r="A5" s="84">
         <v>4</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" t="s" s="85">
         <v>180</v>
       </c>
-      <c r="C5" s="86" t="s">
+      <c r="C5" t="s" s="86">
         <v>181</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" t="s" s="43">
         <v>175</v>
       </c>
       <c r="E5" s="43"/>
-      <c r="F5" s="42" t="s">
+      <c r="F5" t="s" s="42">
         <v>183</v>
       </c>
-      <c r="G5" s="42" t="s">
-        <v>167</v>
-      </c>
+      <c r="G5" s="42"/>
       <c r="H5" s="75"/>
     </row>
   </sheetData>
@@ -3436,380 +3501,379 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="87" style="2" customWidth="1"/>
-    <col min="4" max="4" width="38.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.85546875" style="1" customWidth="1"/>
     <col min="5" max="6" width="33" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="32">
         <v>6</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" t="s" s="33">
         <v>9</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" t="s" s="33">
         <v>2</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" t="s" s="33">
         <v>3</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" t="s" s="33">
         <v>4</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" t="s" s="34">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2" s="125">
+    <row r="2" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="A2" s="152">
         <v>1</v>
       </c>
       <c r="B2" s="66">
         <v>20</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" t="s" s="21">
         <v>31</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" t="s" s="31">
         <v>32</v>
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="35"/>
     </row>
-    <row r="3" spans="1:6" ht="54" x14ac:dyDescent="0.2">
-      <c r="A3" s="125"/>
+    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="A3" s="152"/>
       <c r="B3" s="64">
         <v>20</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" t="s" s="21">
         <v>33</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" t="s" s="31">
         <v>34</v>
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="35"/>
     </row>
-    <row r="4" spans="1:6" ht="54" x14ac:dyDescent="0.2">
-      <c r="A4" s="125"/>
+    <row r="4" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="A4" s="152"/>
       <c r="B4" s="65">
         <v>20</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" t="s" s="21">
         <v>35</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" t="s" s="31">
         <v>36</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="35"/>
     </row>
-    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="A5" s="125"/>
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="152"/>
       <c r="B5" s="66">
         <v>30</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" t="s" s="21">
         <v>37</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" t="s" s="31">
         <v>38</v>
       </c>
       <c r="E5" s="21"/>
       <c r="F5" s="35"/>
     </row>
-    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A6" s="125"/>
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="152"/>
       <c r="B6" s="64">
         <v>30</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" t="s" s="21">
         <v>39</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>40</v>
+      <c r="D6" s="31">
+        <v>23</v>
       </c>
       <c r="E6" s="21"/>
       <c r="F6" s="35"/>
     </row>
-    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="A7" s="126"/>
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="153"/>
       <c r="B7" s="67">
         <v>30</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" t="s" s="38">
         <v>41</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" t="s" s="39">
         <v>42</v>
       </c>
       <c r="E7" s="38"/>
       <c r="F7" s="36"/>
     </row>
-    <row r="8" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A8" s="127">
+    <row r="8" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="A8" s="154">
         <v>2</v>
       </c>
       <c r="B8" s="64">
         <v>20</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" t="s" s="21">
         <v>43</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" t="s" s="31">
         <v>44</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="35"/>
     </row>
-    <row r="9" spans="1:6" ht="54" x14ac:dyDescent="0.2">
-      <c r="A9" s="127"/>
+    <row r="9" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="A9" s="154"/>
       <c r="B9" s="64">
         <v>20</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" t="s" s="21">
         <v>45</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" t="s" s="31">
         <v>46</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="35"/>
     </row>
-    <row r="10" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A10" s="127"/>
+    <row r="10" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="A10" s="154"/>
       <c r="B10" s="64">
         <v>20</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" t="s" s="21">
         <v>47</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" t="s" s="31">
         <v>48</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="35"/>
     </row>
-    <row r="11" spans="1:6" ht="54" x14ac:dyDescent="0.2">
-      <c r="A11" s="127"/>
+    <row r="11" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="A11" s="154"/>
       <c r="B11" s="64">
         <v>30</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" t="s" s="21">
         <v>49</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>19</v>
+      <c r="D11" s="31">
+        <v>5</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="35"/>
     </row>
-    <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="A12" s="127"/>
+    <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="A12" s="154"/>
       <c r="B12" s="64">
         <v>30</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" t="s" s="21">
         <v>50</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" t="s" s="31">
         <v>51</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="35"/>
     </row>
-    <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="A13" s="128"/>
+    <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="A13" s="155"/>
       <c r="B13" s="67">
         <v>30</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" t="s" s="38">
         <v>52</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" t="s" s="39">
         <v>53</v>
       </c>
       <c r="E13" s="38"/>
       <c r="F13" s="36"/>
     </row>
-    <row r="14" spans="1:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="A14" s="127">
+    <row r="14" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="154">
         <v>3</v>
       </c>
       <c r="B14" s="64">
         <v>20</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" t="s" s="21">
         <v>54</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" t="s" s="31">
         <v>55</v>
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="35"/>
     </row>
-    <row r="15" spans="1:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="A15" s="127"/>
+    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="154"/>
       <c r="B15" s="64">
         <v>20</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" t="s" s="21">
         <v>56</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" t="s" s="31">
         <v>57</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="35"/>
     </row>
-    <row r="16" spans="1:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="A16" s="127"/>
+    <row r="16" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="A16" s="154"/>
       <c r="B16" s="64">
         <v>20</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" t="s" s="21">
         <v>58</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" t="s" s="31">
         <v>59</v>
       </c>
       <c r="E16" s="21"/>
       <c r="F16" s="35"/>
     </row>
-    <row r="17" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A17" s="127"/>
+    <row r="17" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="154"/>
       <c r="B17" s="64">
         <v>30</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" t="s" s="21">
         <v>60</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" t="s" s="31">
         <v>61</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="35"/>
     </row>
-    <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A18" s="127"/>
+    <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="A18" s="154"/>
       <c r="B18" s="64">
         <v>30</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" t="s" s="21">
         <v>84</v>
       </c>
-      <c r="D18" s="31" t="s">
-        <v>62</v>
+      <c r="D18" s="31">
+        <v>852</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="35"/>
     </row>
-    <row r="19" spans="1:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="A19" s="128"/>
+    <row r="19" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="A19" s="155"/>
       <c r="B19" s="67">
         <v>30</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" t="s" s="38">
         <v>63</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" t="s" s="39">
         <v>64</v>
       </c>
       <c r="E19" s="38"/>
       <c r="F19" s="36"/>
     </row>
-    <row r="20" spans="1:6" ht="54" x14ac:dyDescent="0.2">
-      <c r="A20" s="127">
+    <row r="20" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="A20" s="154">
         <v>4</v>
       </c>
       <c r="B20" s="64">
         <v>20</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" t="s" s="21">
         <v>65</v>
       </c>
-      <c r="D20" s="31" t="s">
-        <v>66</v>
+      <c r="D20" s="31">
+        <v>42</v>
       </c>
       <c r="E20" s="21"/>
       <c r="F20" s="35"/>
     </row>
-    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A21" s="127"/>
+    <row r="21" spans="1:6" ht="108" x14ac:dyDescent="0.25">
+      <c r="A21" s="154"/>
       <c r="B21" s="64">
         <v>20</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" t="s" s="21">
         <v>67</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" t="s" s="31">
         <v>68</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="35"/>
     </row>
-    <row r="22" spans="1:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="A22" s="127"/>
+    <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="154"/>
       <c r="B22" s="64">
         <v>20</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" t="s" s="21">
         <v>69</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" t="s" s="31">
         <v>70</v>
       </c>
       <c r="E22" s="21"/>
       <c r="F22" s="35"/>
     </row>
-    <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="A23" s="127"/>
+    <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="A23" s="154"/>
       <c r="B23" s="64">
         <v>30</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" t="s" s="21">
         <v>71</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" t="s" s="31">
         <v>72</v>
       </c>
       <c r="E23" s="21"/>
       <c r="F23" s="35"/>
     </row>
-    <row r="24" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A24" s="127"/>
+    <row r="24" spans="1:6" ht="108" x14ac:dyDescent="0.25">
+      <c r="A24" s="154"/>
       <c r="B24" s="64">
         <v>30</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" t="s" s="21">
         <v>73</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" t="s" s="31">
         <v>74</v>
       </c>
       <c r="E24" s="21"/>
       <c r="F24" s="35"/>
     </row>
-    <row r="25" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="129"/>
+    <row r="25" spans="1:6" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="156"/>
       <c r="B25" s="68">
         <v>30</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C25" t="s" s="43">
         <v>75</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" t="s" s="44">
         <v>76</v>
       </c>
       <c r="E25" s="43"/>
@@ -3831,72 +3895,71 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
     <col min="2" max="2" width="73" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="34.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="34.42578125" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="57">
         <v>0</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" t="s" s="58">
         <v>2</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" t="s" s="59">
         <v>3</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" t="s" s="59">
         <v>4</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" t="s" s="60">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="54" x14ac:dyDescent="0.25">
       <c r="A2" s="61">
         <v>1</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" t="s" s="51">
         <v>77</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" t="s" s="40">
         <v>78</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.25">
       <c r="A3" s="62">
         <v>2</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" t="s" s="53">
         <v>79</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" t="s" s="31">
         <v>80</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:5" ht="54.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="63">
         <v>3</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="B4" t="s" s="85">
         <v>81</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" t="s" s="44">
         <v>82</v>
       </c>
       <c r="D4" s="95"/>
@@ -3905,4 +3968,135 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38038B57-C186-44D2-8B40-F948EDCE938F}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="118"/>
+    <col min="2" max="2" width="30.85546875" style="118" customWidth="1"/>
+    <col min="3" max="7" width="16.42578125" style="118" customWidth="1"/>
+    <col min="8" max="8" width="37.28515625" style="118" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="118" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="118"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s" s="119">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="123">
+        <v>184</v>
+      </c>
+      <c r="C1" t="s" s="125">
+        <v>185</v>
+      </c>
+      <c r="D1" t="s" s="125">
+        <v>186</v>
+      </c>
+      <c r="E1" t="s" s="127">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s" s="127">
+        <v>188</v>
+      </c>
+      <c r="G1" t="s" s="127">
+        <v>189</v>
+      </c>
+      <c r="H1" t="s" s="126">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="120">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="128">
+        <v>194</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137">
+        <v>1</v>
+      </c>
+      <c r="H2" s="132"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="121">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="129">
+        <v>40</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139">
+        <v>2</v>
+      </c>
+      <c r="H3" s="133"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="124">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="130">
+        <v>195</v>
+      </c>
+      <c r="C4" s="89"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="141">
+        <v>3</v>
+      </c>
+      <c r="H4" s="134"/>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="122">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="131">
+        <v>196</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="142"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143">
+        <v>4</v>
+      </c>
+      <c r="H5" s="135"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E0CD4C-6834-47C8-9134-8D220797B185}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="118"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>